<commit_message>
Corrected voltage regulator connections and added level shifters to inputs to BLE112.
</commit_message>
<xml_diff>
--- a/Hardware/BOM/Bluegiga_BLE112_XBee_Module_BOM.xlsx
+++ b/Hardware/BOM/Bluegiga_BLE112_XBee_Module_BOM.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>Id</t>
   </si>
@@ -85,75 +85,30 @@
     <t>AAT3221IGV-3.3-T1</t>
   </si>
   <si>
-    <t>603-BLE112-A</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>873-AAT3221IGV-33T1</t>
-  </si>
-  <si>
     <t>Skyworks Solutions, Inc.</t>
   </si>
   <si>
-    <t>150mA NanoPower LDO Linear Regulator</t>
-  </si>
-  <si>
     <t>BLE112-A</t>
   </si>
   <si>
     <t>Bluegiga Technologies</t>
   </si>
   <si>
-    <t>BLE Module 4.0 SINGLEMODE W/ANT</t>
-  </si>
-  <si>
-    <t>81-GRM39R105K6.3</t>
-  </si>
-  <si>
     <t>GRM188R60J105KA01D</t>
   </si>
   <si>
-    <t>SMD/SMT 0603 1uF 6.3volts X5R 10%</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
-    <t>F981A225MMA</t>
-  </si>
-  <si>
-    <t>Nichicon</t>
-  </si>
-  <si>
-    <t>CAP TANT 2.2UF 10V 20% 0603</t>
-  </si>
-  <si>
-    <t>647-F981A225MMA</t>
-  </si>
-  <si>
-    <t>963-TMK107F474ZA-T</t>
-  </si>
-  <si>
     <t>TMK107F474ZA-T</t>
   </si>
   <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
-    <t>SMD/SMT CAP MLCC 0603 25V Y5V 0.47uF +80/-20%</t>
-  </si>
-  <si>
     <t>0603</t>
   </si>
   <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>0.100"</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -169,7 +124,100 @@
     <t>C6</t>
   </si>
   <si>
-    <t>J2</t>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>609-3695-1-ND</t>
+  </si>
+  <si>
+    <t>20021121-00010C4LF</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>CONN HEADER 10POS DL UNSHRD SMD</t>
+  </si>
+  <si>
+    <t>0.050"</t>
+  </si>
+  <si>
+    <t>BSS138CT-ND</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6</t>
+  </si>
+  <si>
+    <t>541-10KGCT-ND</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 50V 220MA SOT-23</t>
+  </si>
+  <si>
+    <t>Fairchild</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>CRCW060310K0JNEA</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>2.0mm</t>
+  </si>
+  <si>
+    <t>1276-2087-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B475KQ8NQNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics America, Inc</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>1446-1017-1-ND</t>
+  </si>
+  <si>
+    <t>CLASS 2 BLTOOTH 4.0 MODULE</t>
+  </si>
+  <si>
+    <t>863-1491-1-ND</t>
+  </si>
+  <si>
+    <t>490-1550-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 6.3V 10% X5R 0603</t>
+  </si>
+  <si>
+    <t>587-1259-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.47UF 25V Y5V 0603</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.15A SOT23-5</t>
   </si>
 </sst>
 </file>
@@ -228,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -236,6 +284,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,33 +602,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -582,7 +646,7 @@
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -591,12 +655,12 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -611,159 +675,246 @@
       <c r="G2" s="4">
         <v>0.5</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>43</v>
+      <c r="H2" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>38</v>
+      <c r="H3" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>39</v>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>40</v>
+      <c r="H5" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>41</v>
+      <c r="H6" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>35</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="4">
+        <v>6</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Corrected BOM per new 3.3V only design
</commit_message>
<xml_diff>
--- a/Hardware/BOM/Bluegiga_BLE112_XBee_Module_BOM.xlsx
+++ b/Hardware/BOM/Bluegiga_BLE112_XBee_Module_BOM.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Serial_EEPROM_Board2" localSheetId="0">Sheet1!$A$1:$E$7</definedName>
+    <definedName name="Serial_EEPROM_Board2" localSheetId="0">Sheet1!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Id</t>
   </si>
@@ -82,12 +82,6 @@
     <t>CONN HEADER 2MM SINGLE STR 40POS</t>
   </si>
   <si>
-    <t>AAT3221IGV-3.3-T1</t>
-  </si>
-  <si>
-    <t>Skyworks Solutions, Inc.</t>
-  </si>
-  <si>
     <t>BLE112-A</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>C1, C2, C3</t>
   </si>
   <si>
@@ -145,42 +136,6 @@
     <t>0.050"</t>
   </si>
   <si>
-    <t>BSS138CT-ND</t>
-  </si>
-  <si>
-    <t>Q1, Q2, Q3</t>
-  </si>
-  <si>
-    <t>SOT-23-3</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6</t>
-  </si>
-  <si>
-    <t>541-10KGCT-ND</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 50V 220MA SOT-23</t>
-  </si>
-  <si>
-    <t>Fairchild</t>
-  </si>
-  <si>
-    <t>BSS138</t>
-  </si>
-  <si>
-    <t>CRCW060310K0JNEA</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
     <t>2.0mm</t>
   </si>
   <si>
@@ -202,9 +157,6 @@
     <t>CLASS 2 BLTOOTH 4.0 MODULE</t>
   </si>
   <si>
-    <t>863-1491-1-ND</t>
-  </si>
-  <si>
     <t>490-1550-1-ND</t>
   </si>
   <si>
@@ -215,9 +167,6 @@
   </si>
   <si>
     <t>CAP CER 0.47UF 25V Y5V 0603</t>
-  </si>
-  <si>
-    <t>IC REG LDO 3.3V 0.15A SOT23-5</t>
   </si>
 </sst>
 </file>
@@ -276,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -296,7 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +553,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,10 +624,10 @@
         <v>0.5</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -687,229 +635,142 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>57</v>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="H7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="4">
-        <v>6</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct BOM line numbering.  Also removed 'special' library from project to stop the warning that it couldn't find the library.
</commit_message>
<xml_diff>
--- a/Hardware/BOM/Bluegiga_BLE112_XBee_Module_BOM.xlsx
+++ b/Hardware/BOM/Bluegiga_BLE112_XBee_Module_BOM.xlsx
@@ -556,7 +556,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>40</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>36</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>42</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>30</v>

</xml_diff>